<commit_message>
average yearly change in cpev in place
</commit_message>
<xml_diff>
--- a/data/output/cpev.xlsx
+++ b/data/output/cpev.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="292">
   <si>
     <t>Kommun</t>
   </si>
   <si>
-    <t>ChargingPointsPerYear</t>
+    <t>cpevChangeAverage</t>
   </si>
   <si>
     <t>Ale</t>
@@ -538,6 +538,9 @@
     <t>Oxelösund</t>
   </si>
   <si>
+    <t>Pajala</t>
+  </si>
+  <si>
     <t>Partille</t>
   </si>
   <si>
@@ -547,9 +550,6 @@
     <t>Piteå</t>
   </si>
   <si>
-    <t>Pajala</t>
-  </si>
-  <si>
     <t>Ragunda</t>
   </si>
   <si>
@@ -889,7 +889,7 @@
     <t>Östra Göinge</t>
   </si>
   <si>
-    <t>Övertorneå</t>
+    <t>-inf</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1269,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>0.02244389027431421</v>
+        <v>0.1134787542554533</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1280,7 +1280,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0.03372681281618887</v>
+        <v>0.1837390904915021</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1291,7 +1291,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>0.07174887892376682</v>
+        <v>0.3880669415474169</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1302,7 +1302,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>0.2702702702702703</v>
+        <v>1.457725947521866</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1313,7 +1313,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>0.3564356435643564</v>
+        <v>-24.53682437605267</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1324,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>0.8888888888888888</v>
+        <v>4.968944099378882</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1335,7 +1335,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1.214285714285714</v>
+        <v>-8.637873754152823</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1346,7 +1346,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>0.1239316239316239</v>
+        <v>-7.926123720516244</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1357,7 +1357,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>0.1473684210526316</v>
+        <v>0.7380073800738007</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1368,7 +1368,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>0.02236421725239617</v>
+        <v>-3.221874523868124</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1379,7 +1379,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>0.08163265306122448</v>
+        <v>0.3835091083413231</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1390,7 +1390,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>0.9607843137254902</v>
+        <v>-8.291708291708295</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1412,7 +1412,7 @@
         <v>15</v>
       </c>
       <c r="C15">
-        <v>0.07017543859649122</v>
+        <v>0.3593890386343217</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1423,7 +1423,7 @@
         <v>16</v>
       </c>
       <c r="C16">
-        <v>0.05641025641025641</v>
+        <v>0.2862347124642207</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1434,7 +1434,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>0.01626016260162602</v>
+        <v>0.07459903021260723</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1445,7 +1445,7 @@
         <v>18</v>
       </c>
       <c r="C18">
-        <v>0.2666666666666667</v>
+        <v>0.3552532123960684</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1456,7 +1456,7 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>0.8522727272727273</v>
+        <v>-52.40202275600507</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1467,7 +1467,7 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>0.07544378698224852</v>
+        <v>-5.733691595760561</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1478,7 +1478,7 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>0.1135701805474665</v>
+        <v>0.235429320767496</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1489,7 +1489,7 @@
         <v>22</v>
       </c>
       <c r="C22">
-        <v>0.01199400299850075</v>
+        <v>-0.7600281491907107</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1511,7 +1511,7 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <v>0.125</v>
+        <v>0.6493506493506493</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1521,8 +1521,8 @@
       <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="C25">
-        <v>0.4166666666666667</v>
+      <c r="C25" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1533,7 +1533,7 @@
         <v>26</v>
       </c>
       <c r="C26">
-        <v>0.1923076923076923</v>
+        <v>0.9920634920634922</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1544,7 +1544,7 @@
         <v>27</v>
       </c>
       <c r="C27">
-        <v>0.1851851851851852</v>
+        <v>0.8965929468021518</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1555,7 +1555,7 @@
         <v>28</v>
       </c>
       <c r="C28">
-        <v>0.02941176470588235</v>
+        <v>0.1680672268907563</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1566,7 +1566,7 @@
         <v>29</v>
       </c>
       <c r="C29">
-        <v>0.06551475881929446</v>
+        <v>0.03304247418631744</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1577,7 +1577,7 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>0.2068965517241379</v>
+        <v>0.8614501076812634</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1588,7 +1588,7 @@
         <v>31</v>
       </c>
       <c r="C31">
-        <v>6.5</v>
+        <v>33.33333333333333</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1599,7 +1599,7 @@
         <v>32</v>
       </c>
       <c r="C32">
-        <v>1.129032258064516</v>
+        <v>-19.09254267744834</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1610,7 +1610,7 @@
         <v>33</v>
       </c>
       <c r="C33">
-        <v>0.01240694789081886</v>
+        <v>-0.4698773448773448</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1621,7 +1621,7 @@
         <v>34</v>
       </c>
       <c r="C34">
-        <v>0.06289308176100629</v>
+        <v>-2.514559780746831</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1632,7 +1632,7 @@
         <v>35</v>
       </c>
       <c r="C35">
-        <v>0.25</v>
+        <v>1.470588235294118</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1643,7 +1643,7 @@
         <v>36</v>
       </c>
       <c r="C36">
-        <v>0.1069306930693069</v>
+        <v>-0.8362928170466263</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1654,7 +1654,7 @@
         <v>37</v>
       </c>
       <c r="C37">
-        <v>0.09690553745928339</v>
+        <v>0.2238999371642903</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1665,7 +1665,7 @@
         <v>38</v>
       </c>
       <c r="C38">
-        <v>0.009259259259259259</v>
+        <v>0.04746084480303749</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1676,7 +1676,7 @@
         <v>39</v>
       </c>
       <c r="C39">
-        <v>0.2285714285714286</v>
+        <v>1.038961038961039</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1687,7 +1687,7 @@
         <v>40</v>
       </c>
       <c r="C40">
-        <v>0.03623188405797102</v>
+        <v>0.2232142857142857</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1698,7 +1698,7 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>0.271523178807947</v>
+        <v>-2.940669289217007</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1709,7 +1709,7 @@
         <v>42</v>
       </c>
       <c r="C42">
-        <v>0.04651162790697674</v>
+        <v>0.2727582679849983</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1720,7 +1720,7 @@
         <v>43</v>
       </c>
       <c r="C43">
-        <v>0.1794117647058824</v>
+        <v>-5.171447495796607</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1731,7 +1731,7 @@
         <v>44</v>
       </c>
       <c r="C44">
-        <v>0.3555555555555556</v>
+        <v>1.889020070838253</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1742,7 +1742,7 @@
         <v>45</v>
       </c>
       <c r="C45">
-        <v>0.1267605633802817</v>
+        <v>0.545950864422202</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1753,7 +1753,7 @@
         <v>46</v>
       </c>
       <c r="C46">
-        <v>0.08247422680412371</v>
+        <v>0.3582624272279444</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1783,7 +1783,7 @@
         <v>49</v>
       </c>
       <c r="C49">
-        <v>0.06060606060606061</v>
+        <v>0.2801120448179272</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1794,7 +1794,7 @@
         <v>50</v>
       </c>
       <c r="C50">
-        <v>0.04878048780487805</v>
+        <v>-4.529616724738675</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1805,7 +1805,7 @@
         <v>51</v>
       </c>
       <c r="C51">
-        <v>0.1196808510638298</v>
+        <v>-3.70728562217924</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1816,7 +1816,7 @@
         <v>52</v>
       </c>
       <c r="C52">
-        <v>0.02298850574712644</v>
+        <v>0.09398496240601503</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1827,7 +1827,7 @@
         <v>53</v>
       </c>
       <c r="C53">
-        <v>0.04191616766467066</v>
+        <v>-4.770642201834862</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1838,7 +1838,7 @@
         <v>54</v>
       </c>
       <c r="C54">
-        <v>0.4388185654008439</v>
+        <v>-14.0272373894743</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1849,7 +1849,7 @@
         <v>55</v>
       </c>
       <c r="C55">
-        <v>0.5600000000000001</v>
+        <v>2.941176470588234</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1871,7 +1871,7 @@
         <v>57</v>
       </c>
       <c r="C57">
-        <v>0.03125</v>
+        <v>0.1443001443001443</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1882,7 +1882,7 @@
         <v>58</v>
       </c>
       <c r="C58">
-        <v>0.5042016806722689</v>
+        <v>3.139717425431711</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1893,7 +1893,7 @@
         <v>59</v>
       </c>
       <c r="C59">
-        <v>0.2025431425976385</v>
+        <v>-2.828091716744887</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1904,7 +1904,7 @@
         <v>60</v>
       </c>
       <c r="C60">
-        <v>0.152317880794702</v>
+        <v>0.0241965236612863</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1926,7 +1926,7 @@
         <v>62</v>
       </c>
       <c r="C62">
-        <v>0.03555555555555556</v>
+        <v>0.2096985583224115</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1937,7 +1937,7 @@
         <v>63</v>
       </c>
       <c r="C63">
-        <v>0.1090909090909091</v>
+        <v>0.6211180124223601</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1948,7 +1948,7 @@
         <v>64</v>
       </c>
       <c r="C64">
-        <v>0.1509433962264151</v>
+        <v>0.7469654528478058</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1959,7 +1959,7 @@
         <v>65</v>
       </c>
       <c r="C65">
-        <v>0.04195804195804196</v>
+        <v>0.2016806722689076</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1970,7 +1970,7 @@
         <v>66</v>
       </c>
       <c r="C66">
-        <v>0.1405797101449275</v>
+        <v>-2.4448718965654</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1981,7 +1981,7 @@
         <v>67</v>
       </c>
       <c r="C67">
-        <v>0.0196078431372549</v>
+        <v>0.1540238737004236</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1992,7 +1992,7 @@
         <v>68</v>
       </c>
       <c r="C68">
-        <v>0.03189300411522634</v>
+        <v>-0.8054680897345835</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2003,7 +2003,7 @@
         <v>69</v>
       </c>
       <c r="C69">
-        <v>0.8205128205128205</v>
+        <v>4.664723032069971</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2014,7 +2014,7 @@
         <v>70</v>
       </c>
       <c r="C70">
-        <v>0.09333333333333334</v>
+        <v>0.3610108303249097</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2025,7 +2025,7 @@
         <v>71</v>
       </c>
       <c r="C71">
-        <v>0.09677419354838709</v>
+        <v>0.4595940252776714</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2036,7 +2036,7 @@
         <v>72</v>
       </c>
       <c r="C72">
-        <v>0.3067454455933038</v>
+        <v>0.8587004474695912</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2047,7 +2047,7 @@
         <v>73</v>
       </c>
       <c r="C73">
-        <v>0.07058823529411765</v>
+        <v>0.322234156820623</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2058,7 +2058,7 @@
         <v>74</v>
       </c>
       <c r="C74">
-        <v>0.1153846153846154</v>
+        <v>-5.140946010511229</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2080,7 +2080,7 @@
         <v>76</v>
       </c>
       <c r="C76">
-        <v>0.05399408284023668</v>
+        <v>-0.2311083949300617</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2091,7 +2091,7 @@
         <v>77</v>
       </c>
       <c r="C77">
-        <v>0.08076009501187649</v>
+        <v>-0.4372152238005897</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2102,7 +2102,7 @@
         <v>78</v>
       </c>
       <c r="C78">
-        <v>0.1818181818181818</v>
+        <v>-6.039239730226854</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2113,7 +2113,7 @@
         <v>79</v>
       </c>
       <c r="C79">
-        <v>0.03092783505154639</v>
+        <v>0.1674107142857143</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2124,7 +2124,7 @@
         <v>80</v>
       </c>
       <c r="C80">
-        <v>0.2608695652173913</v>
+        <v>1.08499095840868</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2135,7 +2135,7 @@
         <v>81</v>
       </c>
       <c r="C81">
-        <v>1.54</v>
+        <v>-63.84236453201969</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2146,7 +2146,7 @@
         <v>82</v>
       </c>
       <c r="C82">
-        <v>0.2807017543859649</v>
+        <v>-2.404610071820512</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2157,7 +2157,7 @@
         <v>83</v>
       </c>
       <c r="C83">
-        <v>0.2009646302250804</v>
+        <v>-3.93968966052979</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2168,7 +2168,7 @@
         <v>84</v>
       </c>
       <c r="C84">
-        <v>0.04054054054054054</v>
+        <v>-0.7788469901715044</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2179,7 +2179,7 @@
         <v>85</v>
       </c>
       <c r="C85">
-        <v>0.01517450682852807</v>
+        <v>0.1148369315571888</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2190,7 +2190,7 @@
         <v>86</v>
       </c>
       <c r="C86">
-        <v>0.193452380952381</v>
+        <v>0.8826724606192287</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2201,7 +2201,7 @@
         <v>87</v>
       </c>
       <c r="C87">
-        <v>0.2173913043478261</v>
+        <v>1.133786848072562</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2212,7 +2212,7 @@
         <v>88</v>
       </c>
       <c r="C88">
-        <v>0.04761904761904762</v>
+        <v>0.2415458937198068</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2223,7 +2223,7 @@
         <v>89</v>
       </c>
       <c r="C89">
-        <v>0.06060606060606061</v>
+        <v>-1.668634395907123</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2234,7 +2234,7 @@
         <v>90</v>
       </c>
       <c r="C90">
-        <v>0.4782608695652174</v>
+        <v>3.666666666666667</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2245,7 +2245,7 @@
         <v>91</v>
       </c>
       <c r="C91">
-        <v>0.04007820136852395</v>
+        <v>0.200655801889101</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2256,7 +2256,7 @@
         <v>92</v>
       </c>
       <c r="C92">
-        <v>0.06687898089171974</v>
+        <v>-0.8694313205591402</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2267,7 +2267,7 @@
         <v>93</v>
       </c>
       <c r="C93">
-        <v>0.1428571428571428</v>
+        <v>0.9398496240601504</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2278,7 +2278,7 @@
         <v>94</v>
       </c>
       <c r="C94">
-        <v>0.08631772268135904</v>
+        <v>-1.140095357177208</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2300,7 +2300,7 @@
         <v>96</v>
       </c>
       <c r="C96">
-        <v>0.1044776119402985</v>
+        <v>-1.691890057685783</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2311,7 +2311,7 @@
         <v>97</v>
       </c>
       <c r="C97">
-        <v>0.05555555555555555</v>
+        <v>-7.613869470833086</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2322,7 +2322,7 @@
         <v>98</v>
       </c>
       <c r="C98">
-        <v>0.1286624203821656</v>
+        <v>-3.750590018699054</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2333,7 +2333,7 @@
         <v>99</v>
       </c>
       <c r="C99">
-        <v>0.1307339449541284</v>
+        <v>-2.019262375912169</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2344,7 +2344,7 @@
         <v>100</v>
       </c>
       <c r="C100">
-        <v>0.1134969325153374</v>
+        <v>-3.906720916214586</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2355,7 +2355,7 @@
         <v>101</v>
       </c>
       <c r="C101">
-        <v>0.04166666666666666</v>
+        <v>0.2463054187192118</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2366,7 +2366,7 @@
         <v>102</v>
       </c>
       <c r="C102">
-        <v>0.05737704918032787</v>
+        <v>0.3105590062111801</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2377,7 +2377,7 @@
         <v>103</v>
       </c>
       <c r="C103">
-        <v>0.1229508196721311</v>
+        <v>0.6802721088435374</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2388,7 +2388,7 @@
         <v>104</v>
       </c>
       <c r="C104">
-        <v>0.09345794392523364</v>
+        <v>0.4001600640256103</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2399,7 +2399,7 @@
         <v>105</v>
       </c>
       <c r="C105">
-        <v>0.01049868766404199</v>
+        <v>0.06144393241167435</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2410,7 +2410,7 @@
         <v>106</v>
       </c>
       <c r="C106">
-        <v>0.1428571428571428</v>
+        <v>0.7595676307332749</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2421,7 +2421,7 @@
         <v>107</v>
       </c>
       <c r="C107">
-        <v>0.09738134206219312</v>
+        <v>-1.778969378119519</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2432,7 +2432,7 @@
         <v>108</v>
       </c>
       <c r="C108">
-        <v>0.1728395061728395</v>
+        <v>-1.922563417890521</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2443,7 +2443,7 @@
         <v>109</v>
       </c>
       <c r="C109">
-        <v>0.375</v>
+        <v>-13.81696428571429</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2454,7 +2454,7 @@
         <v>110</v>
       </c>
       <c r="C110">
-        <v>0.06912442396313365</v>
+        <v>0.350140056022409</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2465,7 +2465,7 @@
         <v>111</v>
       </c>
       <c r="C111">
-        <v>0.0529045643153527</v>
+        <v>-0.2402128166441674</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2476,7 +2476,7 @@
         <v>112</v>
       </c>
       <c r="C112">
-        <v>0.1739130434782609</v>
+        <v>0.8086253369272237</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2487,7 +2487,7 @@
         <v>113</v>
       </c>
       <c r="C113">
-        <v>0.0282021151586369</v>
+        <v>-0.3206824523438944</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2498,7 +2498,7 @@
         <v>114</v>
       </c>
       <c r="C114">
-        <v>0.06704980842911877</v>
+        <v>-4.282562031852775</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2509,7 +2509,7 @@
         <v>115</v>
       </c>
       <c r="C115">
-        <v>0.09004739336492891</v>
+        <v>-4.294729940168838</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2520,7 +2520,7 @@
         <v>116</v>
       </c>
       <c r="C116">
-        <v>0.2350993377483444</v>
+        <v>-3.216202402248914</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2531,7 +2531,7 @@
         <v>117</v>
       </c>
       <c r="C117">
-        <v>0.05913978494623656</v>
+        <v>-0.9145449224465906</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2542,7 +2542,7 @@
         <v>118</v>
       </c>
       <c r="C118">
-        <v>0.2727272727272727</v>
+        <v>1.21580547112462</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2553,7 +2553,7 @@
         <v>119</v>
       </c>
       <c r="C119">
-        <v>0.02</v>
+        <v>0.1066098081023454</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2564,7 +2564,7 @@
         <v>120</v>
       </c>
       <c r="C120">
-        <v>0.3008130081300813</v>
+        <v>-11.72850958565244</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2575,7 +2575,7 @@
         <v>121</v>
       </c>
       <c r="C121">
-        <v>0.03125</v>
+        <v>0.1563416064100059</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2586,7 +2586,7 @@
         <v>122</v>
       </c>
       <c r="C122">
-        <v>0.2</v>
+        <v>0.9984639016897082</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2597,7 +2597,7 @@
         <v>123</v>
       </c>
       <c r="C123">
-        <v>0.02209944751381215</v>
+        <v>-0.2735736204296042</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2608,7 +2608,7 @@
         <v>124</v>
       </c>
       <c r="C124">
-        <v>0.07868383404864092</v>
+        <v>-0.8196072220462465</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2630,7 +2630,7 @@
         <v>126</v>
       </c>
       <c r="C126">
-        <v>0.1929824561403509</v>
+        <v>0.8928571428571428</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2641,7 +2641,7 @@
         <v>127</v>
       </c>
       <c r="C127">
-        <v>0.1607680722891566</v>
+        <v>0.1105887557117913</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2652,7 +2652,7 @@
         <v>128</v>
       </c>
       <c r="C128">
-        <v>0.2689655172413793</v>
+        <v>-5.756929637526653</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2663,7 +2663,7 @@
         <v>129</v>
       </c>
       <c r="C129">
-        <v>0.09090909090909091</v>
+        <v>0.4880212954747116</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2674,7 +2674,7 @@
         <v>130</v>
       </c>
       <c r="C130">
-        <v>0.2</v>
+        <v>-25.50724637681159</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2685,7 +2685,7 @@
         <v>131</v>
       </c>
       <c r="C131">
-        <v>0.04018912529550828</v>
+        <v>-0.8605955717428458</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2696,7 +2696,7 @@
         <v>132</v>
       </c>
       <c r="C132">
-        <v>0.1759259259259259</v>
+        <v>-0.3578743613405659</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2707,7 +2707,7 @@
         <v>133</v>
       </c>
       <c r="C133">
-        <v>0.09081632653061225</v>
+        <v>-1.713808330349684</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2718,7 +2718,7 @@
         <v>134</v>
       </c>
       <c r="C134">
-        <v>0.1516471549142391</v>
+        <v>0.4823827846435098</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2729,7 +2729,7 @@
         <v>135</v>
       </c>
       <c r="C135">
-        <v>0.5892857142857143</v>
+        <v>3.466386554621849</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2740,7 +2740,7 @@
         <v>136</v>
       </c>
       <c r="C136">
-        <v>0.06177606177606178</v>
+        <v>0.3835091083413231</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2751,7 +2751,7 @@
         <v>137</v>
       </c>
       <c r="C137">
-        <v>0.06592624234657554</v>
+        <v>-0.8576892094226599</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2762,7 +2762,7 @@
         <v>138</v>
       </c>
       <c r="C138">
-        <v>0.8920863309352518</v>
+        <v>-42.00546360276394</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2773,7 +2773,7 @@
         <v>139</v>
       </c>
       <c r="C139">
-        <v>0.3636363636363636</v>
+        <v>6.349206349206349</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2784,7 +2784,7 @@
         <v>140</v>
       </c>
       <c r="C140">
-        <v>0.09705882352941177</v>
+        <v>-1.998382811597551</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2795,7 +2795,7 @@
         <v>141</v>
       </c>
       <c r="C141">
-        <v>0.0045662100456621</v>
+        <v>0.02484472049689441</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2806,7 +2806,7 @@
         <v>142</v>
       </c>
       <c r="C142">
-        <v>0.3974358974358974</v>
+        <v>1.860744297719088</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2817,7 +2817,7 @@
         <v>143</v>
       </c>
       <c r="C143">
-        <v>0.4567901234567901</v>
+        <v>2.826585179526356</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2828,7 +2828,7 @@
         <v>144</v>
       </c>
       <c r="C144">
-        <v>0.09831460674157304</v>
+        <v>0.505050505050505</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2839,7 +2839,7 @@
         <v>145</v>
       </c>
       <c r="C145">
-        <v>0.166023166023166</v>
+        <v>-11.54156577885391</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2850,7 +2850,7 @@
         <v>146</v>
       </c>
       <c r="C146">
-        <v>0.0321285140562249</v>
+        <v>-0.7821862922384144</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2861,7 +2861,7 @@
         <v>147</v>
       </c>
       <c r="C147">
-        <v>0.3809523809523809</v>
+        <v>-4.923717059639389</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2872,7 +2872,7 @@
         <v>148</v>
       </c>
       <c r="C148">
-        <v>0.08943089430894309</v>
+        <v>-22.32804232804233</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2894,7 +2894,7 @@
         <v>150</v>
       </c>
       <c r="C150">
-        <v>0.05562130177514793</v>
+        <v>-1.058003653919028</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2905,7 +2905,7 @@
         <v>151</v>
       </c>
       <c r="C151">
-        <v>0.25</v>
+        <v>1.051329622758194</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2916,7 +2916,7 @@
         <v>152</v>
       </c>
       <c r="C152">
-        <v>0.07446808510638298</v>
+        <v>0.4319654427645789</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2927,7 +2927,7 @@
         <v>153</v>
       </c>
       <c r="C153">
-        <v>0.05468341182626897</v>
+        <v>0.189219237733033</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2938,7 +2938,7 @@
         <v>154</v>
       </c>
       <c r="C154">
-        <v>0.2261904761904762</v>
+        <v>1.012793176972282</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2960,7 +2960,7 @@
         <v>156</v>
       </c>
       <c r="C156">
-        <v>0.07142857142857142</v>
+        <v>0.3861003861003861</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2971,7 +2971,7 @@
         <v>157</v>
       </c>
       <c r="C157">
-        <v>0.09090909090909091</v>
+        <v>0.5592841163310962</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2982,7 +2982,7 @@
         <v>158</v>
       </c>
       <c r="C158">
-        <v>0.09596928982725528</v>
+        <v>-0.370907984390613</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2993,7 +2993,7 @@
         <v>159</v>
       </c>
       <c r="C159">
-        <v>0.0800561797752809</v>
+        <v>-2.570871554196592</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -3004,7 +3004,7 @@
         <v>160</v>
       </c>
       <c r="C160">
-        <v>0.04878048780487805</v>
+        <v>0.3663003663003663</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -3015,7 +3015,7 @@
         <v>161</v>
       </c>
       <c r="C161">
-        <v>0.0291970802919708</v>
+        <v>0.1511715797430083</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -3026,7 +3026,7 @@
         <v>162</v>
       </c>
       <c r="C162">
-        <v>0.05384615384615385</v>
+        <v>0.2469135802469136</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3037,7 +3037,7 @@
         <v>163</v>
       </c>
       <c r="C163">
-        <v>0.09121621621621621</v>
+        <v>-1.60522707106558</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3048,7 +3048,7 @@
         <v>164</v>
       </c>
       <c r="C164">
-        <v>0.07818930041152264</v>
+        <v>0.3314146171289029</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3059,7 +3059,7 @@
         <v>165</v>
       </c>
       <c r="C165">
-        <v>0.1024258760107817</v>
+        <v>0.5972025774005972</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3070,7 +3070,7 @@
         <v>166</v>
       </c>
       <c r="C166">
-        <v>0.8918918918918919</v>
+        <v>5.124223602484456</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3081,7 +3081,7 @@
         <v>167</v>
       </c>
       <c r="C167">
-        <v>0.3373493975903614</v>
+        <v>-14.6667795749005</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3092,7 +3092,7 @@
         <v>168</v>
       </c>
       <c r="C168">
-        <v>0.375</v>
+        <v>-7.557885539536915</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3103,7 +3103,7 @@
         <v>169</v>
       </c>
       <c r="C169">
-        <v>0.1736526946107785</v>
+        <v>0.1710189452124934</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3114,7 +3114,7 @@
         <v>170</v>
       </c>
       <c r="C170">
-        <v>0.0396039603960396</v>
+        <v>0.1937046004842615</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3125,7 +3125,7 @@
         <v>171</v>
       </c>
       <c r="C171">
-        <v>0.3435897435897436</v>
+        <v>1.676257192894671</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3136,7 +3136,7 @@
         <v>172</v>
       </c>
       <c r="C172">
-        <v>0.05882352941176471</v>
+        <v>0.2435064935064935</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3158,7 +3158,7 @@
         <v>174</v>
       </c>
       <c r="C174">
-        <v>0.006791171477079796</v>
+        <v>3.03951367781155</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3169,7 +3169,7 @@
         <v>175</v>
       </c>
       <c r="C175">
-        <v>0.6571428571428571</v>
+        <v>0.03573662110247476</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3180,7 +3180,7 @@
         <v>176</v>
       </c>
       <c r="C176">
-        <v>0.08888888888888889</v>
+        <v>2.671312427409988</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3191,7 +3191,7 @@
         <v>177</v>
       </c>
       <c r="C177">
-        <v>0.4166666666666667</v>
+        <v>-0.5619282831498962</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3199,10 +3199,10 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C178">
-        <v>0.6666666666666666</v>
+        <v>3.03951367781155</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3210,10 +3210,10 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C179">
-        <v>0.1176470588235294</v>
+        <v>3.174603174603174</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3221,10 +3221,10 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C180">
-        <v>0.2051282051282051</v>
+        <v>0.7011393514461</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3232,10 +3232,10 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C181">
-        <v>0.1333333333333333</v>
+        <v>-10.55770325751446</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3243,10 +3243,10 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C182">
-        <v>0.07894736842105263</v>
+        <v>-5.415735198673109</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3254,10 +3254,10 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C183">
-        <v>0</v>
+        <v>-2.755257354083186</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3265,10 +3265,10 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C184">
-        <v>0.642570281124498</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3276,10 +3276,10 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C185">
-        <v>0.5076142131979695</v>
+        <v>2.980070776680946</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3287,10 +3287,10 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C186">
-        <v>0.1373626373626374</v>
+        <v>-27.00295189005676</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3298,10 +3298,10 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C187">
-        <v>0.1</v>
+        <v>-13.64567332309268</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3309,10 +3309,10 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C188">
-        <v>0.05963302752293578</v>
+        <v>0.5123568414707654</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3320,10 +3320,10 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C189">
-        <v>0.1075268817204301</v>
+        <v>0.3550942365473914</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3331,10 +3331,10 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C190">
-        <v>0</v>
+        <v>0.6312732782021337</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3342,10 +3342,10 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C191">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3353,10 +3353,10 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C192">
-        <v>0.1481826654240447</v>
+        <v>0.2070393374741201</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3364,10 +3364,10 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C193">
-        <v>0.7466666666666667</v>
+        <v>0.2779702306454496</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3375,10 +3375,10 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C194">
-        <v>0.2027972027972028</v>
+        <v>3.149606299212598</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3386,10 +3386,10 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C195">
-        <v>0.01194239550403934</v>
+        <v>-5.775577557755777</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3397,10 +3397,10 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C196">
-        <v>0.03523035230352303</v>
+        <v>0.06123478135581011</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3408,10 +3408,10 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C197">
-        <v>4.666666666666667</v>
+        <v>0.1218046816728906</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3419,10 +3419,10 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C198">
-        <v>0.25</v>
+        <v>-60.00000000000001</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3430,10 +3430,10 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C199">
-        <v>0</v>
+        <v>1.217329036877909</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3441,10 +3441,10 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C200">
-        <v>0.05947136563876652</v>
+        <v>-3.061224489795918</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3452,10 +3452,10 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C201">
-        <v>0.1048328172297415</v>
+        <v>-0.9489417738016047</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3463,10 +3463,10 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C202">
-        <v>0.1</v>
+        <v>-1.029289781728238</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3474,10 +3474,10 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C203">
-        <v>2.157894736842105</v>
+        <v>0.5882352941176471</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3485,10 +3485,10 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C204">
-        <v>0.1811594202898551</v>
+        <v>9.601873536299767</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3496,10 +3496,10 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C205">
-        <v>1.422018348623853</v>
+        <v>0.7855048177628823</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3507,10 +3507,10 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C206">
-        <v>0.7428571428571429</v>
+        <v>-10.93027600056041</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3518,10 +3518,10 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C207">
-        <v>0.004245283018867924</v>
+        <v>1.712614870509608</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3529,10 +3529,10 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C208">
-        <v>0.1306772908366534</v>
+        <v>-0.3303693810845956</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3540,10 +3540,10 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C209">
-        <v>0.09278350515463918</v>
+        <v>-8.74622666856321</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3551,10 +3551,10 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C210">
-        <v>0</v>
+        <v>-23.31879316612142</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3562,10 +3562,10 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C211">
-        <v>0.1574803149606299</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3573,10 +3573,10 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C212">
-        <v>0.04262295081967213</v>
+        <v>0.8186655751125667</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3584,10 +3584,10 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C213">
-        <v>0</v>
+        <v>0.2393225331369661</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3595,10 +3595,10 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C214">
-        <v>0.1119402985074627</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3606,10 +3606,10 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C215">
-        <v>0.1075268817204301</v>
+        <v>0.6979990693345742</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3617,10 +3617,10 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C216">
-        <v>0.1521739130434783</v>
+        <v>-3.590714636370012</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3628,10 +3628,10 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C217">
-        <v>0.1737089201877934</v>
+        <v>0.7905138339920948</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3639,10 +3639,10 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C218">
-        <v>0.1973684210526316</v>
+        <v>0.9973045822102425</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3650,10 +3650,10 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C219">
-        <v>0.02054794520547945</v>
+        <v>-6.285714285714286</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3661,10 +3661,10 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C220">
-        <v>0.05806451612903226</v>
+        <v>-0.8465253276006262</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3672,10 +3672,10 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C221">
-        <v>0.8861788617886179</v>
+        <v>-5.747737326684695</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3683,10 +3683,10 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C222">
-        <v>0.03418803418803419</v>
+        <v>-6.888381888381888</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3694,10 +3694,10 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C223">
-        <v>0.05376344086021505</v>
+        <v>0.1943634596695821</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3705,10 +3705,10 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C224">
-        <v>0.05147058823529412</v>
+        <v>-3.287981859410431</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3716,10 +3716,10 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C225">
-        <v>0.05649717514124294</v>
+        <v>0.228310502283105</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3727,10 +3727,10 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C226">
-        <v>0.1142857142857143</v>
+        <v>-9.211894364732791</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3738,10 +3738,10 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C227">
-        <v>0.01809954751131222</v>
+        <v>0.5733397037744864</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3749,10 +3749,10 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C228">
-        <v>0.1238095238095238</v>
+        <v>0.08873114463176575</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3760,10 +3760,10 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C229">
-        <v>0.71</v>
+        <v>0.5952380952380952</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3771,10 +3771,10 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C230">
-        <v>0.04347826086956522</v>
+        <v>4.390847247990104</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3782,10 +3782,10 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C231">
-        <v>0.02419354838709677</v>
+        <v>0.2070393374741201</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3793,10 +3793,10 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C232">
-        <v>0.1158536585365854</v>
+        <v>0.1302648719062093</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3804,10 +3804,10 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C233">
-        <v>0.1203501094091904</v>
+        <v>0.5160239000543182</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3815,10 +3815,10 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C234">
-        <v>0.09048938134810711</v>
+        <v>-3.993880657285746</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3826,10 +3826,10 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C235">
-        <v>0.09302325581395349</v>
+        <v>-2.796107013987724</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3837,10 +3837,10 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C236">
-        <v>0.01298701298701299</v>
+        <v>-5.324232081911263</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3848,10 +3848,10 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C237">
-        <v>0.04567307692307692</v>
+        <v>-1.270532001602497</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3859,10 +3859,10 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C238">
-        <v>0.05333333333333334</v>
+        <v>-0.00207700600254735</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3870,10 +3870,10 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C239">
-        <v>0.141091658084449</v>
+        <v>0.2991772625280479</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3881,10 +3881,10 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C240">
-        <v>0.2518248175182482</v>
+        <v>-2.834247487689818</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3892,10 +3892,10 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C241">
-        <v>0.09335038363171355</v>
+        <v>-4.483681112894597</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3903,10 +3903,10 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C242">
-        <v>0.1428571428571428</v>
+        <v>-1.363482671174979</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3914,10 +3914,10 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C243">
-        <v>0.07560137457044673</v>
+        <v>-1.506042499114093</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3925,10 +3925,10 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C244">
-        <v>0.1555891238670695</v>
+        <v>0.3230069006019674</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3936,10 +3936,10 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C245">
-        <v>0.02409638554216868</v>
+        <v>-0.5257455105341863</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3947,10 +3947,10 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C246">
-        <v>0.07228915662650602</v>
+        <v>0.1236858379715523</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3958,10 +3958,10 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C247">
-        <v>0.05970149253731343</v>
+        <v>0.3631961259079903</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3969,10 +3969,10 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C248">
-        <v>0.06382978723404255</v>
+        <v>0.2528445006321112</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3980,10 +3980,10 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C249">
-        <v>0.03094777562862669</v>
+        <v>0.2764976958525346</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3991,10 +3991,10 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C250">
-        <v>0.1714285714285714</v>
+        <v>0.1351693841344936</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -4002,10 +4002,10 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C251">
-        <v>0.1495726495726496</v>
+        <v>0.8928571428571428</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -4013,10 +4013,10 @@
         <v>250</v>
       </c>
       <c r="B252" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C252">
-        <v>0.1189979123173278</v>
+        <v>-7.701863354037266</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -4024,10 +4024,10 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C253">
-        <v>0.009433962264150943</v>
+        <v>-2.922541229184641</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -4035,10 +4035,10 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C254">
-        <v>0.07117008443908324</v>
+        <v>0.04195510803440319</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -4046,10 +4046,10 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C255">
-        <v>0.06906077348066299</v>
+        <v>0.374936451448907</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -4057,10 +4057,10 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C256">
-        <v>0.2631578947368421</v>
+        <v>0.3924646781789639</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -4068,10 +4068,10 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C257">
-        <v>0.1344086021505376</v>
+        <v>1.19047619047619</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -4079,10 +4079,10 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C258">
-        <v>0.2105263157894737</v>
+        <v>-0.4999590197524793</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -4090,10 +4090,10 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C259">
-        <v>0.0303030303030303</v>
+        <v>1.228878648233487</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -4101,10 +4101,10 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C260">
-        <v>0.04672897196261682</v>
+        <v>0.1287001287001287</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -4112,10 +4112,10 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C261">
-        <v>0.2298850574712644</v>
+        <v>0.322234156820623</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -4123,10 +4123,10 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C262">
-        <v>0.1116816431322208</v>
+        <v>1.185536455245999</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -4134,10 +4134,10 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C263">
-        <v>0.07974481658692185</v>
+        <v>-0.7034505370284128</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -4145,10 +4145,10 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C264">
-        <v>0.1751824817518248</v>
+        <v>-2.306971006431923</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -4156,10 +4156,10 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C265">
-        <v>0.1219739292364991</v>
+        <v>0.8701957940536621</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -4167,10 +4167,10 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C266">
-        <v>0.09399684044233807</v>
+        <v>-0.7746830388339823</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -4178,10 +4178,10 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C267">
-        <v>0.03603603603603604</v>
+        <v>-6.385255261783572</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -4189,10 +4189,10 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C268">
-        <v>0</v>
+        <v>0.15527950310559</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -4200,10 +4200,10 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C269">
-        <v>0.2170087976539589</v>
+        <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -4211,10 +4211,10 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C270">
-        <v>0.03097345132743363</v>
+        <v>1.01161995898838</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -4222,10 +4222,10 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C271">
-        <v>1.875</v>
+        <v>0.1680672268907563</v>
       </c>
     </row>
     <row r="272" spans="1:3">
@@ -4233,10 +4233,10 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>272</v>
-      </c>
-      <c r="C272">
-        <v>0</v>
+        <v>271</v>
+      </c>
+      <c r="C272" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -4244,10 +4244,10 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C273">
-        <v>0.3478260869565217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:3">
@@ -4255,10 +4255,10 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C274">
-        <v>0.1506622516556291</v>
+        <v>1.970443349753695</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -4266,10 +4266,10 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C275">
-        <v>0.04697986577181208</v>
+        <v>0.8160703075957313</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -4277,10 +4277,10 @@
         <v>274</v>
       </c>
       <c r="B276" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C276">
-        <v>0.4680851063829787</v>
+        <v>-1.370113262696383</v>
       </c>
     </row>
     <row r="277" spans="1:3">
@@ -4288,10 +4288,10 @@
         <v>275</v>
       </c>
       <c r="B277" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C277">
-        <v>1.089285714285714</v>
+        <v>-9.246031746031745</v>
       </c>
     </row>
     <row r="278" spans="1:3">
@@ -4299,10 +4299,10 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C278">
-        <v>0.9137931034482759</v>
+        <v>-6.199111769059956</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -4310,10 +4310,10 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C279">
-        <v>0.2222222222222222</v>
+        <v>-137.7065111758989</v>
       </c>
     </row>
     <row r="280" spans="1:3">
@@ -4321,10 +4321,10 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C280">
-        <v>0.05128205128205128</v>
+        <v>2.051282051282051</v>
       </c>
     </row>
     <row r="281" spans="1:3">
@@ -4332,10 +4332,10 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C281">
-        <v>0</v>
+        <v>0.2455996725337699</v>
       </c>
     </row>
     <row r="282" spans="1:3">
@@ -4343,10 +4343,10 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C282">
-        <v>0</v>
+        <v>-14.28571428571428</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -4354,10 +4354,10 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C283">
-        <v>0.3958333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:3">
@@ -4365,10 +4365,10 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>284</v>
-      </c>
-      <c r="C284">
-        <v>0.091773656680932</v>
+        <v>283</v>
+      </c>
+      <c r="C284" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="285" spans="1:3">
@@ -4376,10 +4376,10 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C285">
-        <v>0.2</v>
+        <v>-0.05253258428828252</v>
       </c>
     </row>
     <row r="286" spans="1:3">
@@ -4387,10 +4387,10 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C286">
-        <v>0.1039182282793867</v>
+        <v>-20.27506654835847</v>
       </c>
     </row>
     <row r="287" spans="1:3">
@@ -4398,10 +4398,10 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C287">
-        <v>0.3302263648468708</v>
+        <v>-1.255894762968479</v>
       </c>
     </row>
     <row r="288" spans="1:3">
@@ -4409,10 +4409,10 @@
         <v>286</v>
       </c>
       <c r="B288" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C288">
-        <v>0.02724177071509648</v>
+        <v>-6.510110893672538</v>
       </c>
     </row>
     <row r="289" spans="1:3">
@@ -4420,10 +4420,10 @@
         <v>287</v>
       </c>
       <c r="B289" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C289">
-        <v>0.04430379746835443</v>
+        <v>0.1342957864696995</v>
       </c>
     </row>
     <row r="290" spans="1:3">
@@ -4431,10 +4431,10 @@
         <v>288</v>
       </c>
       <c r="B290" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C290">
-        <v>0.0202020202020202</v>
+        <v>0.1886792452830189</v>
       </c>
     </row>
     <row r="291" spans="1:3">
@@ -4442,10 +4442,10 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C291">
-        <v>0.1111111111111111</v>
+        <v>0.08900756564307971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>